<commit_message>
updated report system in the framework
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium Projects\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D12051A-E5F9-4E7E-9211-3A989723C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AutomationExercise" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">TestCaseName </t>
+  </si>
+  <si>
+    <t>TC01_RegisterNewUser</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>gauravma0r5@gmail.com</t>
+  </si>
+  <si>
+    <t>Gaurav Manral</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +57,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +116,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +423,269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F9A8B8E8-0B1B-4F5A-8F4C-68397C50688F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;L_x000D_&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022B C2 - Restricted use </oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c5e6e129-f928-4a05-ae32-d838f6b21bdd}" enabled="1" method="Standard" siteId="{8b87af7d-8647-4dc7-8df4-5f69a2011bb5}" contentBits="3" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
updated fetching test data functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium Projects\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D12051A-E5F9-4E7E-9211-3A989723C18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D9BE12-863B-42EC-9D5C-908F65AFAD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="3435" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AutomationExercise" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">TestCaseName </t>
   </si>
@@ -43,6 +43,33 @@
   </si>
   <si>
     <t>Gaurav Manral</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -427,7 +454,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,15 +474,33 @@
       <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>